<commit_message>
Szombati munka, ikonok, karakter kepernyo
</commit_message>
<xml_diff>
--- a/designDocs/game_design01.xlsx
+++ b/designDocs/game_design01.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ALAP_ELEMEK" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
-    <sheet name="Munka3" sheetId="3" r:id="rId3"/>
+    <sheet name="képernyők" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Játékos</t>
   </si>
@@ -55,13 +56,97 @@
   </si>
   <si>
     <t xml:space="preserve">Alapéterlmezett jelszó: </t>
+  </si>
+  <si>
+    <t>imgUrl</t>
+  </si>
+  <si>
+    <t>tblstats</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>statid</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>primary key</t>
+  </si>
+  <si>
+    <t>Kezdőképernyő</t>
+  </si>
+  <si>
+    <t>Erőforrások</t>
+  </si>
+  <si>
+    <t>Karakter</t>
+  </si>
+  <si>
+    <t>Gyártás</t>
+  </si>
+  <si>
+    <t>Kutatás</t>
+  </si>
+  <si>
+    <t>Hős portrés</t>
+  </si>
+  <si>
+    <t>Hős statok</t>
+  </si>
+  <si>
+    <t>A HŐS KÉPE</t>
+  </si>
+  <si>
+    <t>not null</t>
+  </si>
+  <si>
+    <t>not null default(1)</t>
+  </si>
+  <si>
+    <t>not null default(100)</t>
+  </si>
+  <si>
+    <t>not null  default(20)</t>
+  </si>
+  <si>
+    <t>not null, default(20)</t>
+  </si>
+  <si>
+    <t>statname</t>
+  </si>
+  <si>
+    <t>statdesc</t>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+  </si>
+  <si>
+    <t>statinitval</t>
+  </si>
+  <si>
+    <t>statdefval</t>
+  </si>
+  <si>
+    <t>statmaxval</t>
+  </si>
+  <si>
+    <t>statikon</t>
+  </si>
+  <si>
+    <t>not null default('/GAME001/pix/ui/staticons/001.jpg')</t>
+  </si>
+  <si>
+    <t>Felszerelés</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,8 +173,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,8 +194,20 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -125,17 +230,406 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ellenőrzőcella" xfId="1" builtinId="23"/>
@@ -149,6 +643,454 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Egyenes összekötő nyíllal 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1123950" y="1314450"/>
+          <a:ext cx="581025" cy="1885950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Egyenes összekötő nyíllal 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2409826" y="1209675"/>
+          <a:ext cx="1647824" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Téglalap 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3505200" y="3152775"/>
+          <a:ext cx="2171700" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="2000"/>
+            <a:t>STAT1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Téglalap 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3524250" y="3981450"/>
+          <a:ext cx="2171700" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="2000"/>
+            <a:t>STAT2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Téglalap 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="4772025"/>
+          <a:ext cx="2171700" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="2000"/>
+            <a:t>...</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Téglalap 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="907677" y="5793441"/>
+          <a:ext cx="4762500" cy="1165412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="2000"/>
+            <a:t>               STATMEGNEVEZÉS:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="2000" baseline="0"/>
+            <a:t>   STATÉRTÉK</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1400" baseline="0"/>
+            <a:t>stat leírása</a:t>
+          </a:r>
+          <a:endParaRPr lang="hu-HU" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>11207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>672354</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Lekerekített téglalap 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="974912" y="5972736"/>
+          <a:ext cx="907677" cy="784412"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1100"/>
+            <a:t>STAT IKON</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403411</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Egyenes összekötő nyíllal 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2308412" y="3765176"/>
+          <a:ext cx="1456764" cy="2185148"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +1391,13 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +1405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -467,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -475,30 +1421,149 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="I4" t="str">
+        <f>"CREATE TABLE  "&amp; F4 &amp; " ( "</f>
+        <v xml:space="preserve">CREATE TABLE  tblstats ( </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="str">
+        <f xml:space="preserve"> F5 &amp; " " &amp; G5 &amp; " " &amp; H5 &amp; ","</f>
+        <v>statid int primary key,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="str">
+        <f xml:space="preserve"> F6 &amp; " " &amp; G6 &amp; " " &amp; H6 &amp; ","</f>
+        <v>statname varchar(100) not null,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="str">
+        <f xml:space="preserve"> F7 &amp; " " &amp; G7 &amp; " " &amp; H7 &amp; ","</f>
+        <v>statdesc varchar(500) not null default(1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" ref="I8:I11" si="0" xml:space="preserve"> F8 &amp; " " &amp; G8 &amp; " " &amp; H8 &amp; ","</f>
+        <v>statinitval int not null default(100),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>statdefval int not null, default(20),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>statmaxval int not null  default(20),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>statikon varchar(100) not null default('/GAME001/pix/ui/staticons/001.jpg'),</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <f>I4&amp;I5&amp;I6&amp;I7&amp;I8&amp;I9&amp;I10&amp;I11&amp;");"</f>
+        <v>CREATE TABLE  tblstats ( statid int primary key,statname varchar(100) not null,statdesc varchar(500) not null default(1),statinitval int not null default(100),statdefval int not null, default(20),statmaxval int not null  default(20),statikon varchar(100) not null default('/GAME001/pix/ui/staticons/001.jpg'),);</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -508,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -532,12 +1597,445 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:AD29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="G2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="34"/>
+      <c r="L2" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="34"/>
+      <c r="Q2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="34"/>
+      <c r="V2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="34"/>
+      <c r="AA2" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="34"/>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="7"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="7"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="7"/>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="10"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="10"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="10"/>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="10"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="10"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="10"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="10"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="10"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="10"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="10"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="10"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="10"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="10"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="10"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="10"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="10"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="10"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="10"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="10"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="10"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="10"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="10"/>
+    </row>
+    <row r="10" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="13"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="13"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="13"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="K15" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="29"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="29"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="10"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="29"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="29"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="10"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="29"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="29"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
+    </row>
+    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="29"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="29"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="29"/>
+    </row>
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="B15:D29"/>
+    <mergeCell ref="F15:I29"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="K15:L15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stat tábla első rekordjai
</commit_message>
<xml_diff>
--- a/designDocs/game_design01.xlsx
+++ b/designDocs/game_design01.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ALAP_ELEMEK" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
     <sheet name="képernyők" sheetId="3" r:id="rId3"/>
+    <sheet name="Rekordok" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>Játékos</t>
   </si>
@@ -140,13 +140,148 @@
   </si>
   <si>
     <t>Felszerelés</t>
+  </si>
+  <si>
+    <t>usrid</t>
+  </si>
+  <si>
+    <t>loginname</t>
+  </si>
+  <si>
+    <t>usermail</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>char(128)</t>
+  </si>
+  <si>
+    <t>not null default(C70B5DD9EBFB6F51D09D4132B7170C9D20750A7852F00680F65658F0310E810056E6763C34C9A00B0E940076F54495C169FC2302CCEB312039271C43469507DC)</t>
+  </si>
+  <si>
+    <t>usrstatid</t>
+  </si>
+  <si>
+    <t>FKEY(tblusers.usrid)</t>
+  </si>
+  <si>
+    <t>FKEY(tblstats.statid)</t>
+  </si>
+  <si>
+    <t>statval</t>
+  </si>
+  <si>
+    <t>tblusrstats</t>
+  </si>
+  <si>
+    <t>insigned bigint</t>
+  </si>
+  <si>
+    <t>Ennyi életerőpontod, van amit elveszíthetsz, mielőtt meghalna a karaktered.</t>
+  </si>
+  <si>
+    <t>/GAME001/pix/ui/icons/eletero_icon128.jpg</t>
+  </si>
+  <si>
+    <t>Varázserő</t>
+  </si>
+  <si>
+    <t>Varázslataiadet ebből táplálhatod, ha értéke 0 nem tudsz varázsolni.</t>
+  </si>
+  <si>
+    <t>Munkakaedv</t>
+  </si>
+  <si>
+    <t>Ha nincs munkakedv nincs munka. A gyártás ezt az erőforrást használja</t>
+  </si>
+  <si>
+    <t>Vitalitás</t>
+  </si>
+  <si>
+    <t>Testi eddzettséges, ami nüveli az életerőpontok számát.</t>
+  </si>
+  <si>
+    <t>Növeli a varászerő pontok számát, és a varázslatok hatékonyságát.</t>
+  </si>
+  <si>
+    <t>Kreativitás</t>
+  </si>
+  <si>
+    <t>A maximális munkaerőt fejleszti</t>
+  </si>
+  <si>
+    <t>tblskills</t>
+  </si>
+  <si>
+    <t>skillid</t>
+  </si>
+  <si>
+    <t>skillname</t>
+  </si>
+  <si>
+    <t>skildesc</t>
+  </si>
+  <si>
+    <t>skillVal</t>
+  </si>
+  <si>
+    <t>skillMax</t>
+  </si>
+  <si>
+    <t>skillrequ</t>
+  </si>
+  <si>
+    <t>skillIkon</t>
+  </si>
+  <si>
+    <t>Védelem</t>
+  </si>
+  <si>
+    <t>Támadás</t>
+  </si>
+  <si>
+    <t>tblskilltypes</t>
+  </si>
+  <si>
+    <t>skillTpId</t>
+  </si>
+  <si>
+    <t>skillTpName</t>
+  </si>
+  <si>
+    <t>FK_skillTpId</t>
+  </si>
+  <si>
+    <t>Mindenre kis befolyással van az akciók sikerétől a ritka erőforrások megtalálásáig.</t>
+  </si>
+  <si>
+    <t>Mennyire vagy védett az ellenfelek által okozott sérülések ellen.</t>
+  </si>
+  <si>
+    <t>Mennyire sikeres a támadások az ellenfelek ellen.</t>
+  </si>
+  <si>
+    <t>Kritikus esély</t>
+  </si>
+  <si>
+    <t>Mekkora esélyed van a kritikus sikerre harcban, vagy gyártásban-</t>
+  </si>
+  <si>
+    <t>Kritikus mennyiség</t>
+  </si>
+  <si>
+    <t>Mennyivel nagyobb a kritikus találat/siker esetén a sérülés/haladás.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +316,25 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +358,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -536,12 +693,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -560,6 +746,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
@@ -615,24 +816,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Ellenőrzőcella" xfId="1" builtinId="23"/>
+    <cellStyle name="Jegyzet" xfId="2" builtinId="10"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,6 +848,152 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Egyenes összekötő nyíllal 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1209675" y="933450"/>
+          <a:ext cx="3305175" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Egyenes összekötő nyíllal 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1200150" y="2286000"/>
+          <a:ext cx="3276600" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Egyenes összekötő nyíllal 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1447800" y="3533775"/>
+          <a:ext cx="3171826" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1380,17 +1728,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48.5703125" bestFit="1" customWidth="1"/>
@@ -1421,7 +1770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1509,7 +1858,7 @@
         <v>statinitval int not null default(100),</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1524,7 +1873,11 @@
         <v>statdefval int not null, default(20),</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="F10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1539,7 +1892,13 @@
         <v>statmaxval int not null  default(20),</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
@@ -1554,18 +1913,212 @@
         <v>statikon varchar(100) not null default('/GAME001/pix/ui/staticons/001.jpg'),</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" t="str">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="str">
         <f>I4&amp;I5&amp;I6&amp;I7&amp;I8&amp;I9&amp;I10&amp;I11&amp;");"</f>
         <v>CREATE TABLE  tblstats ( statid int primary key,statname varchar(100) not null,statdesc varchar(500) not null default(1),statinitval int not null default(100),statdefval int not null, default(20),statmaxval int not null  default(20),statikon varchar(100) not null default('/GAME001/pix/ui/staticons/001.jpg'),);</v>
       </c>
     </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1599,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -1610,30 +2163,30 @@
   <sheetData>
     <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="G2" s="33" t="s">
+      <c r="C2" s="16"/>
+      <c r="G2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="L2" s="33" t="s">
+      <c r="H2" s="16"/>
+      <c r="L2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="Q2" s="33" t="s">
+      <c r="M2" s="16"/>
+      <c r="Q2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="V2" s="33" t="s">
+      <c r="R2" s="16"/>
+      <c r="V2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="34"/>
-      <c r="AA2" s="33" t="s">
+      <c r="W2" s="16"/>
+      <c r="AA2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="34"/>
+      <c r="AB2" s="16"/>
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -1663,10 +2216,10 @@
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="10"/>
@@ -1693,8 +2246,8 @@
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="10"/>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -1719,8 +2272,8 @@
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="10"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -1745,8 +2298,8 @@
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="10"/>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
@@ -1849,193 +2402,1243 @@
     </row>
     <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="K15" s="33" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="K15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="34"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
       <c r="K17" s="8"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="29"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
       <c r="K18" s="8"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="29"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
       <c r="K19" s="8"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
       <c r="K22" s="8"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="29"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
       <c r="K23" s="11"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
       <c r="N23" s="13"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="29"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="34"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="B15:D29"/>
     <mergeCell ref="F15:I29"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="K15:L15"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" t="str">
+        <f>"INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES("</f>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES(</v>
+      </c>
+      <c r="J1" t="str">
+        <f>B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;")"</f>
+        <v>statdesc,statinitval,statdefval,statmaxval,statikon)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"'"</f>
+        <v>'</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"',"</f>
+        <v>',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="41">
+        <v>150</v>
+      </c>
+      <c r="D3" s="41">
+        <v>100</v>
+      </c>
+      <c r="E3" s="42">
+        <v>0</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="str">
+        <f>$G$1&amp;$G$2&amp;A3&amp;$H$2&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3</f>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Életerő','Ennyi életerőpontod, van amit elveszíthetsz, mielőtt meghalna a karaktered.','150','100','0','/GAME001/pix/ui/icons/eletero_icon128.jpg');</v>
+      </c>
+      <c r="H3" t="str">
+        <f>$G$2&amp;B3&amp;$H$2</f>
+        <v>'Ennyi életerőpontod, van amit elveszíthetsz, mielőtt meghalna a karaktered.',</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:M3" si="0">$G$2&amp;C3&amp;$H$2</f>
+        <v>'150',</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>'100',</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>'0',</v>
+      </c>
+      <c r="L3" t="str">
+        <f>$G$2&amp;F3&amp;"');"</f>
+        <v>'/GAME001/pix/ui/icons/eletero_icon128.jpg');</v>
+      </c>
+      <c r="M3" t="str">
+        <f>G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3</f>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Életerő','Ennyi életerőpontod, van amit elveszíthetsz, mielőtt meghalna a karaktered.','150','100','0','/GAME001/pix/ui/icons/eletero_icon128.jpg');'Ennyi életerőpontod, van amit elveszíthetsz, mielőtt meghalna a karaktered.','150','100','0','/GAME001/pix/ui/icons/eletero_icon128.jpg');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="41">
+        <v>100</v>
+      </c>
+      <c r="D4" s="41">
+        <v>50</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G13" si="1">$G$1&amp;$G$2&amp;A4&amp;$H$2&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4</f>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Varázserő','Varázslataiadet ebből táplálhatod, ha értéke 0 nem tudsz varázsolni.','100','50','0','');</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H13" si="2">$G$2&amp;B4&amp;$H$2</f>
+        <v>'Varázslataiadet ebből táplálhatod, ha értéke 0 nem tudsz varázsolni.',</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I13" si="3">$G$2&amp;C4&amp;$H$2</f>
+        <v>'100',</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J13" si="4">$G$2&amp;D4&amp;$H$2</f>
+        <v>'50',</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K13" si="5">$G$2&amp;E4&amp;$H$2</f>
+        <v>'0',</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L13" si="6">$G$2&amp;F4&amp;"');"</f>
+        <v>'');</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M13" si="7">G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4</f>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Varázserő','Varázslataiadet ebből táplálhatod, ha értéke 0 nem tudsz varázsolni.','100','50','0','');'Varázslataiadet ebből táplálhatod, ha értéke 0 nem tudsz varázsolni.','100','50','0','');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="41">
+        <v>100</v>
+      </c>
+      <c r="D5" s="41">
+        <v>50</v>
+      </c>
+      <c r="E5" s="42">
+        <v>0</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Munkakaedv','Ha nincs munkakedv nincs munka. A gyártás ezt az erőforrást használja','100','50','0','');</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>'Ha nincs munkakedv nincs munka. A gyártás ezt az erőforrást használja',</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="3"/>
+        <v>'100',</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="4"/>
+        <v>'50',</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="5"/>
+        <v>'0',</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Munkakaedv','Ha nincs munkakedv nincs munka. A gyártás ezt az erőforrást használja','100','50','0','');'Ha nincs munkakedv nincs munka. A gyártás ezt az erőforrást használja','100','50','0','');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="41">
+        <v>10</v>
+      </c>
+      <c r="D6" s="41">
+        <v>10</v>
+      </c>
+      <c r="E6" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Vitalitás','Testi eddzettséges, ami nüveli az életerőpontok számát.','10','10','50000','');</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>'Testi eddzettséges, ami nüveli az életerőpontok számát.',</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="3"/>
+        <v>'10',</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="4"/>
+        <v>'10',</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Vitalitás','Testi eddzettséges, ami nüveli az életerőpontok számát.','10','10','50000','');'Testi eddzettséges, ami nüveli az életerőpontok számát.','10','10','50000','');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="41">
+        <v>10</v>
+      </c>
+      <c r="D7" s="41">
+        <v>10</v>
+      </c>
+      <c r="E7" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Intelligencia','Növeli a varászerő pontok számát, és a varázslatok hatékonyságát.','10','10','50000','');</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>'Növeli a varászerő pontok számát, és a varázslatok hatékonyságát.',</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v>'10',</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="4"/>
+        <v>'10',</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Intelligencia','Növeli a varászerő pontok számát, és a varázslatok hatékonyságát.','10','10','50000','');'Növeli a varászerő pontok számát, és a varázslatok hatékonyságát.','10','10','50000','');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="41">
+        <v>10</v>
+      </c>
+      <c r="D8" s="41">
+        <v>10</v>
+      </c>
+      <c r="E8" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kreativitás','A maximális munkaerőt fejleszti','10','10','50000','');</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>'A maximális munkaerőt fejleszti',</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v>'10',</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="4"/>
+        <v>'10',</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kreativitás','A maximális munkaerőt fejleszti','10','10','50000','');'A maximális munkaerőt fejleszti','10','10','50000','');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="41">
+        <v>1</v>
+      </c>
+      <c r="E9" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Szerencse','Mindenre kis befolyással van az akciók sikerétől a ritka erőforrások megtalálásáig.','1','1','50000','');</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>'Mindenre kis befolyással van az akciók sikerétől a ritka erőforrások megtalálásáig.',</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="3"/>
+        <v>'1',</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="4"/>
+        <v>'1',</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Szerencse','Mindenre kis befolyással van az akciók sikerétől a ritka erőforrások megtalálásáig.','1','1','50000','');'Mindenre kis befolyással van az akciók sikerétől a ritka erőforrások megtalálásáig.','1','1','50000','');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="41">
+        <v>1</v>
+      </c>
+      <c r="D10" s="41">
+        <v>1</v>
+      </c>
+      <c r="E10" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Védelem','Mennyire vagy védett az ellenfelek által okozott sérülések ellen.','1','1','50000','');</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>'Mennyire vagy védett az ellenfelek által okozott sérülések ellen.',</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v>'1',</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="4"/>
+        <v>'1',</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Védelem','Mennyire vagy védett az ellenfelek által okozott sérülések ellen.','1','1','50000','');'Mennyire vagy védett az ellenfelek által okozott sérülések ellen.','1','1','50000','');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="41">
+        <v>1</v>
+      </c>
+      <c r="D11" s="41">
+        <v>1</v>
+      </c>
+      <c r="E11" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F11" s="41"/>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Támadás','Mennyire sikeres a támadások az ellenfelek ellen.','1','1','50000','');</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>'Mennyire sikeres a támadások az ellenfelek ellen.',</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v>'1',</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="4"/>
+        <v>'1',</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Támadás','Mennyire sikeres a támadások az ellenfelek ellen.','1','1','50000','');'Mennyire sikeres a támadások az ellenfelek ellen.','1','1','50000','');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="41">
+        <v>1</v>
+      </c>
+      <c r="E12" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F12" s="41"/>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kritikus esély','Mekkora esélyed van a kritikus sikerre harcban, vagy gyártásban-','1','1','50000','');</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>'Mekkora esélyed van a kritikus sikerre harcban, vagy gyártásban-',</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v>'1',</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="4"/>
+        <v>'1',</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kritikus esély','Mekkora esélyed van a kritikus sikerre harcban, vagy gyártásban-','1','1','50000','');'Mekkora esélyed van a kritikus sikerre harcban, vagy gyártásban-','1','1','50000','');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="41">
+        <v>1</v>
+      </c>
+      <c r="D13" s="41">
+        <v>1</v>
+      </c>
+      <c r="E13" s="41">
+        <v>50000</v>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kritikus mennyiség','Mennyivel nagyobb a kritikus találat/siker esetén a sérülés/haladás.','1','1','50000','');</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>'Mennyivel nagyobb a kritikus találat/siker esetén a sérülés/haladás.',</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v>'1',</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="4"/>
+        <v>'1',</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="5"/>
+        <v>'50000',</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="6"/>
+        <v>'');</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO gamedb.tblstats (statname,statdesc,statintval,statdefval,statmaxval,ststikon) VALUES('Kritikus mennyiség','Mennyivel nagyobb a kritikus találat/siker esetén a sérülés/haladás.','1','1','50000','');'Mennyivel nagyobb a kritikus találat/siker esetén a sérülés/haladás.','1','1','50000','');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="38"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="38"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="38"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="38"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="38"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="38"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="38"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="38"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="38"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="38"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="38"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="38"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="38"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="38"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="38"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="38"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="38"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="38"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="38"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="38"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="38"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="38"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>